<commit_message>
set every series parameter, slice border for 10%
</commit_message>
<xml_diff>
--- a/YY_report.xlsx
+++ b/YY_report.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\factory\test\YY_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEED9C48-8D96-43CB-A32F-D7618D9C783E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE883A22-0302-4D15-9C3F-F743E53E3CAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表2" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -190,7 +191,7 @@
     <numFmt numFmtId="176" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;?_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -245,6 +246,13 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -302,14 +310,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -595,8 +603,8 @@
   <sheetPr codeName="工作表5"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -621,7 +629,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -634,7 +642,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -660,8 +668,8 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="156" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:5" ht="156" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -673,15 +681,15 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:5" ht="101.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f>2*1.5*2000*8</f>
         <v>48000</v>
       </c>
@@ -689,26 +697,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:5" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
   </sheetData>
@@ -719,4 +727,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B601DD-5DA6-4883-8F54-C46C8BB02A77}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>